<commit_message>
did formatting for pharmacist and edited fucntions
</commit_message>
<xml_diff>
--- a/sc2002/src/main/resources/Appointment_Outcomes.xlsx
+++ b/sc2002/src/main/resources/Appointment_Outcomes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>Patient ID</t>
   </si>
@@ -506,14 +506,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="25.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="22.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="20.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="12.576428571428572"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="12.576428571428572"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="7" width="19.005"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="8" width="25.576428571428572"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="6" width="12.576428571428572"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="6" width="14.576428571428572"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="6" width="22.005"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="6" width="20.290714285714284"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -588,7 +588,7 @@
         <v>16</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>18</v>
@@ -614,7 +614,7 @@
         <v>21</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>22</v>

</xml_diff>